<commit_message>
fixes resource error bug when importing csv's
</commit_message>
<xml_diff>
--- a/ot2_driver/protopiler/test_configs/simple_provided_info.xlsx
+++ b/ot2_driver/protopiler/test_configs/simple_provided_info.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10911"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kyle/github/ot2_driver/ot2_driver/protopiler/example_configs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abestroka/Argonne/ot2_driver/ot2_driver/protopiler/test_configs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDCD19E4-0DE2-164C-8A15-E0819F87E801}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1C82E45-6B58-BE4F-A623-DEB910620E25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="760" windowWidth="22440" windowHeight="16120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="220" yWindow="3300" windowWidth="22440" windowHeight="16120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="103">
   <si>
     <t>Forward Primer</t>
   </si>
@@ -323,6 +323,12 @@
   </si>
   <si>
     <t>Volume</t>
+  </si>
+  <si>
+    <t>B2</t>
+  </si>
+  <si>
+    <t>B9</t>
   </si>
 </sst>
 </file>
@@ -358,10 +364,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -670,44 +674,44 @@
   <dimension ref="A1:E96"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F93" sqref="F93"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="12.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="1" t="s">
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
         <v>5</v>
       </c>
       <c r="E2">
@@ -715,16 +719,16 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+      <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="1" t="s">
+      <c r="C3" t="s">
+        <v>102</v>
+      </c>
+      <c r="D3" t="s">
         <v>7</v>
       </c>
       <c r="E3">
@@ -732,16 +736,16 @@
       </c>
     </row>
     <row r="4" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+      <c r="A4" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="1" t="s">
+      <c r="C4" t="s">
+        <v>101</v>
+      </c>
+      <c r="D4" t="s">
         <v>9</v>
       </c>
       <c r="E4">
@@ -749,16 +753,16 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
+      <c r="A5" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="1" t="s">
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" t="s">
         <v>11</v>
       </c>
       <c r="E5">
@@ -766,16 +770,16 @@
       </c>
     </row>
     <row r="6" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
+      <c r="A6" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" t="s">
         <v>13</v>
       </c>
       <c r="E6">
@@ -783,16 +787,16 @@
       </c>
     </row>
     <row r="7" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
+      <c r="A7" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" t="s">
         <v>15</v>
       </c>
       <c r="E7">
@@ -800,16 +804,16 @@
       </c>
     </row>
     <row r="8" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
+      <c r="A8" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" t="s">
         <v>17</v>
       </c>
       <c r="E8">
@@ -817,16 +821,16 @@
       </c>
     </row>
     <row r="9" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
+      <c r="A9" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" t="s">
         <v>19</v>
       </c>
       <c r="E9">
@@ -834,16 +838,16 @@
       </c>
     </row>
     <row r="10" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
+      <c r="A10" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" t="s">
         <v>21</v>
       </c>
       <c r="E10">
@@ -851,16 +855,16 @@
       </c>
     </row>
     <row r="11" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
+      <c r="A11" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D11" t="s">
         <v>23</v>
       </c>
       <c r="E11">
@@ -868,16 +872,16 @@
       </c>
     </row>
     <row r="12" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
+      <c r="A12" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" t="s">
         <v>24</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D12" t="s">
         <v>25</v>
       </c>
       <c r="E12">
@@ -885,16 +889,16 @@
       </c>
     </row>
     <row r="13" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
+      <c r="A13" t="s">
         <v>26</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" t="s">
         <v>27</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" t="s">
         <v>26</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D13" t="s">
         <v>27</v>
       </c>
       <c r="E13">
@@ -902,16 +906,16 @@
       </c>
     </row>
     <row r="14" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
+      <c r="A14" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" t="s">
         <v>29</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" t="s">
         <v>28</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D14" t="s">
         <v>29</v>
       </c>
       <c r="E14">
@@ -919,16 +923,16 @@
       </c>
     </row>
     <row r="15" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
+      <c r="A15" t="s">
         <v>30</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" t="s">
         <v>31</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" t="s">
         <v>30</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D15" t="s">
         <v>31</v>
       </c>
       <c r="E15">
@@ -936,16 +940,16 @@
       </c>
     </row>
     <row r="16" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
+      <c r="A16" t="s">
         <v>32</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" t="s">
         <v>33</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" t="s">
         <v>32</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D16" t="s">
         <v>33</v>
       </c>
       <c r="E16">
@@ -953,16 +957,16 @@
       </c>
     </row>
     <row r="17" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
+      <c r="A17" t="s">
         <v>34</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" t="s">
         <v>35</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C17" t="s">
         <v>34</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D17" t="s">
         <v>35</v>
       </c>
       <c r="E17">
@@ -970,16 +974,16 @@
       </c>
     </row>
     <row r="18" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
+      <c r="A18" t="s">
         <v>36</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" t="s">
         <v>37</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C18" t="s">
         <v>36</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D18" t="s">
         <v>37</v>
       </c>
       <c r="E18">
@@ -987,16 +991,16 @@
       </c>
     </row>
     <row r="19" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
+      <c r="A19" t="s">
         <v>38</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" t="s">
         <v>39</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C19" t="s">
         <v>38</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D19" t="s">
         <v>39</v>
       </c>
       <c r="E19">
@@ -1004,16 +1008,16 @@
       </c>
     </row>
     <row r="20" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
+      <c r="A20" t="s">
         <v>40</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" t="s">
         <v>41</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C20" t="s">
         <v>40</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="D20" t="s">
         <v>41</v>
       </c>
       <c r="E20">
@@ -1021,16 +1025,16 @@
       </c>
     </row>
     <row r="21" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="1" t="s">
+      <c r="A21" t="s">
         <v>42</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" t="s">
         <v>43</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C21" t="s">
         <v>42</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="D21" t="s">
         <v>43</v>
       </c>
       <c r="E21">
@@ -1038,16 +1042,16 @@
       </c>
     </row>
     <row r="22" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="1" t="s">
+      <c r="A22" t="s">
         <v>44</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" t="s">
         <v>45</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C22" t="s">
         <v>44</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="D22" t="s">
         <v>45</v>
       </c>
       <c r="E22">
@@ -1055,16 +1059,16 @@
       </c>
     </row>
     <row r="23" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="1" t="s">
+      <c r="A23" t="s">
         <v>46</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" t="s">
         <v>47</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="C23" t="s">
         <v>46</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="D23" t="s">
         <v>47</v>
       </c>
       <c r="E23">
@@ -1072,16 +1076,16 @@
       </c>
     </row>
     <row r="24" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="1" t="s">
+      <c r="A24" t="s">
         <v>48</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" t="s">
         <v>49</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C24" t="s">
         <v>48</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="D24" t="s">
         <v>49</v>
       </c>
       <c r="E24">
@@ -1089,16 +1093,16 @@
       </c>
     </row>
     <row r="25" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="1" t="s">
+      <c r="A25" t="s">
         <v>50</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B25" t="s">
         <v>51</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="C25" t="s">
         <v>50</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="D25" t="s">
         <v>51</v>
       </c>
       <c r="E25">
@@ -1106,16 +1110,16 @@
       </c>
     </row>
     <row r="26" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="1" t="s">
+      <c r="A26" t="s">
         <v>52</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B26" t="s">
         <v>53</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="C26" t="s">
         <v>52</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="D26" t="s">
         <v>53</v>
       </c>
       <c r="E26">
@@ -1123,16 +1127,16 @@
       </c>
     </row>
     <row r="27" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="1" t="s">
+      <c r="A27" t="s">
         <v>54</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B27" t="s">
         <v>55</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="C27" t="s">
         <v>56</v>
       </c>
-      <c r="D27" s="1" t="s">
+      <c r="D27" t="s">
         <v>55</v>
       </c>
       <c r="E27">
@@ -1140,16 +1144,16 @@
       </c>
     </row>
     <row r="28" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="1" t="s">
+      <c r="A28" t="s">
         <v>57</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B28" t="s">
         <v>58</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="C28" t="s">
         <v>59</v>
       </c>
-      <c r="D28" s="1" t="s">
+      <c r="D28" t="s">
         <v>60</v>
       </c>
       <c r="E28">
@@ -1157,16 +1161,16 @@
       </c>
     </row>
     <row r="29" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="1" t="s">
+      <c r="A29" t="s">
         <v>61</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B29" t="s">
         <v>62</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="C29" t="s">
         <v>63</v>
       </c>
-      <c r="D29" s="1" t="s">
+      <c r="D29" t="s">
         <v>64</v>
       </c>
       <c r="E29">
@@ -1174,16 +1178,16 @@
       </c>
     </row>
     <row r="30" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="1" t="s">
+      <c r="A30" t="s">
         <v>65</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B30" t="s">
         <v>66</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="C30" t="s">
         <v>67</v>
       </c>
-      <c r="D30" s="1" t="s">
+      <c r="D30" t="s">
         <v>68</v>
       </c>
       <c r="E30">
@@ -1191,16 +1195,16 @@
       </c>
     </row>
     <row r="31" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="1" t="s">
+      <c r="A31" t="s">
         <v>69</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B31" t="s">
         <v>70</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="C31" t="s">
         <v>71</v>
       </c>
-      <c r="D31" s="1" t="s">
+      <c r="D31" t="s">
         <v>72</v>
       </c>
       <c r="E31">
@@ -1208,16 +1212,16 @@
       </c>
     </row>
     <row r="32" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="1" t="s">
+      <c r="A32" t="s">
         <v>73</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B32" t="s">
         <v>74</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="C32" t="s">
         <v>75</v>
       </c>
-      <c r="D32" s="1" t="s">
+      <c r="D32" t="s">
         <v>76</v>
       </c>
       <c r="E32">
@@ -1225,16 +1229,16 @@
       </c>
     </row>
     <row r="33" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="1" t="s">
+      <c r="A33" t="s">
         <v>77</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B33" t="s">
         <v>78</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="C33" t="s">
         <v>79</v>
       </c>
-      <c r="D33" s="1" t="s">
+      <c r="D33" t="s">
         <v>80</v>
       </c>
       <c r="E33">
@@ -1242,16 +1246,16 @@
       </c>
     </row>
     <row r="34" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="1" t="s">
+      <c r="A34" t="s">
         <v>81</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B34" t="s">
         <v>82</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="C34" t="s">
         <v>83</v>
       </c>
-      <c r="D34" s="1" t="s">
+      <c r="D34" t="s">
         <v>84</v>
       </c>
       <c r="E34">
@@ -1259,16 +1263,16 @@
       </c>
     </row>
     <row r="35" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="1" t="s">
+      <c r="A35" t="s">
         <v>85</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B35" t="s">
         <v>86</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="C35" t="s">
         <v>87</v>
       </c>
-      <c r="D35" s="1" t="s">
+      <c r="D35" t="s">
         <v>88</v>
       </c>
       <c r="E35">
@@ -1276,16 +1280,16 @@
       </c>
     </row>
     <row r="36" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="1" t="s">
+      <c r="A36" t="s">
         <v>89</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="B36" t="s">
         <v>90</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="C36" t="s">
         <v>91</v>
       </c>
-      <c r="D36" s="1" t="s">
+      <c r="D36" t="s">
         <v>92</v>
       </c>
       <c r="E36">
@@ -1293,16 +1297,16 @@
       </c>
     </row>
     <row r="37" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="1" t="s">
+      <c r="A37" t="s">
         <v>93</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="B37" t="s">
         <v>94</v>
       </c>
-      <c r="C37" s="1" t="s">
+      <c r="C37" t="s">
         <v>95</v>
       </c>
-      <c r="D37" s="1" t="s">
+      <c r="D37" t="s">
         <v>94</v>
       </c>
       <c r="E37">
@@ -1310,16 +1314,16 @@
       </c>
     </row>
     <row r="38" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="1" t="s">
+      <c r="A38" t="s">
         <v>96</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="B38" t="s">
         <v>92</v>
       </c>
-      <c r="C38" s="1" t="s">
+      <c r="C38" t="s">
         <v>97</v>
       </c>
-      <c r="D38" s="1" t="s">
+      <c r="D38" t="s">
         <v>90</v>
       </c>
       <c r="E38">
@@ -1327,16 +1331,16 @@
       </c>
     </row>
     <row r="39" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="1" t="s">
+      <c r="A39" t="s">
         <v>98</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="B39" t="s">
         <v>88</v>
       </c>
-      <c r="C39" s="1" t="s">
+      <c r="C39" t="s">
         <v>98</v>
       </c>
-      <c r="D39" s="1" t="s">
+      <c r="D39" t="s">
         <v>86</v>
       </c>
       <c r="E39">
@@ -1344,16 +1348,16 @@
       </c>
     </row>
     <row r="40" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="1" t="s">
+      <c r="A40" t="s">
         <v>97</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="B40" t="s">
         <v>84</v>
       </c>
-      <c r="C40" s="1" t="s">
+      <c r="C40" t="s">
         <v>96</v>
       </c>
-      <c r="D40" s="1" t="s">
+      <c r="D40" t="s">
         <v>82</v>
       </c>
       <c r="E40">
@@ -1361,16 +1365,16 @@
       </c>
     </row>
     <row r="41" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="1" t="s">
+      <c r="A41" t="s">
         <v>95</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="B41" t="s">
         <v>80</v>
       </c>
-      <c r="C41" s="1" t="s">
+      <c r="C41" t="s">
         <v>93</v>
       </c>
-      <c r="D41" s="1" t="s">
+      <c r="D41" t="s">
         <v>78</v>
       </c>
       <c r="E41">
@@ -1378,16 +1382,16 @@
       </c>
     </row>
     <row r="42" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="1" t="s">
+      <c r="A42" t="s">
         <v>91</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="B42" t="s">
         <v>76</v>
       </c>
-      <c r="C42" s="1" t="s">
+      <c r="C42" t="s">
         <v>89</v>
       </c>
-      <c r="D42" s="1" t="s">
+      <c r="D42" t="s">
         <v>74</v>
       </c>
       <c r="E42">
@@ -1395,16 +1399,16 @@
       </c>
     </row>
     <row r="43" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="1" t="s">
+      <c r="A43" t="s">
         <v>87</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="B43" t="s">
         <v>72</v>
       </c>
-      <c r="C43" s="1" t="s">
+      <c r="C43" t="s">
         <v>85</v>
       </c>
-      <c r="D43" s="1" t="s">
+      <c r="D43" t="s">
         <v>70</v>
       </c>
       <c r="E43">
@@ -1412,16 +1416,16 @@
       </c>
     </row>
     <row r="44" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="1" t="s">
+      <c r="A44" t="s">
         <v>83</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="B44" t="s">
         <v>68</v>
       </c>
-      <c r="C44" s="1" t="s">
+      <c r="C44" t="s">
         <v>81</v>
       </c>
-      <c r="D44" s="1" t="s">
+      <c r="D44" t="s">
         <v>66</v>
       </c>
       <c r="E44">
@@ -1429,16 +1433,16 @@
       </c>
     </row>
     <row r="45" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="1" t="s">
+      <c r="A45" t="s">
         <v>79</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="B45" t="s">
         <v>64</v>
       </c>
-      <c r="C45" s="1" t="s">
+      <c r="C45" t="s">
         <v>77</v>
       </c>
-      <c r="D45" s="1" t="s">
+      <c r="D45" t="s">
         <v>62</v>
       </c>
       <c r="E45">
@@ -1446,16 +1450,16 @@
       </c>
     </row>
     <row r="46" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="1" t="s">
+      <c r="A46" t="s">
         <v>75</v>
       </c>
-      <c r="B46" s="1" t="s">
+      <c r="B46" t="s">
         <v>60</v>
       </c>
-      <c r="C46" s="1" t="s">
+      <c r="C46" t="s">
         <v>73</v>
       </c>
-      <c r="D46" s="1" t="s">
+      <c r="D46" t="s">
         <v>58</v>
       </c>
       <c r="E46">
@@ -1463,16 +1467,16 @@
       </c>
     </row>
     <row r="47" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="1" t="s">
+      <c r="A47" t="s">
         <v>71</v>
       </c>
-      <c r="B47" s="1" t="s">
+      <c r="B47" t="s">
         <v>56</v>
       </c>
-      <c r="C47" s="1" t="s">
+      <c r="C47" t="s">
         <v>69</v>
       </c>
-      <c r="D47" s="1" t="s">
+      <c r="D47" t="s">
         <v>56</v>
       </c>
       <c r="E47">
@@ -1480,16 +1484,16 @@
       </c>
     </row>
     <row r="48" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="1" t="s">
+      <c r="A48" t="s">
         <v>67</v>
       </c>
-      <c r="B48" s="1" t="s">
+      <c r="B48" t="s">
         <v>59</v>
       </c>
-      <c r="C48" s="1" t="s">
+      <c r="C48" t="s">
         <v>65</v>
       </c>
-      <c r="D48" s="1" t="s">
+      <c r="D48" t="s">
         <v>59</v>
       </c>
       <c r="E48">
@@ -1497,16 +1501,16 @@
       </c>
     </row>
     <row r="49" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="1" t="s">
+      <c r="A49" t="s">
         <v>63</v>
       </c>
-      <c r="B49" s="1" t="s">
+      <c r="B49" t="s">
         <v>63</v>
       </c>
-      <c r="C49" s="1" t="s">
+      <c r="C49" t="s">
         <v>61</v>
       </c>
-      <c r="D49" s="1" t="s">
+      <c r="D49" t="s">
         <v>63</v>
       </c>
       <c r="E49">
@@ -1514,16 +1518,16 @@
       </c>
     </row>
     <row r="50" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="1" t="s">
+      <c r="A50" t="s">
         <v>59</v>
       </c>
-      <c r="B50" s="1" t="s">
+      <c r="B50" t="s">
         <v>67</v>
       </c>
-      <c r="C50" s="1" t="s">
+      <c r="C50" t="s">
         <v>57</v>
       </c>
-      <c r="D50" s="1" t="s">
+      <c r="D50" t="s">
         <v>67</v>
       </c>
       <c r="E50">
@@ -1531,16 +1535,16 @@
       </c>
     </row>
     <row r="51" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="1" t="s">
+      <c r="A51" t="s">
         <v>56</v>
       </c>
-      <c r="B51" s="1" t="s">
+      <c r="B51" t="s">
         <v>71</v>
       </c>
-      <c r="C51" s="1" t="s">
+      <c r="C51" t="s">
         <v>54</v>
       </c>
-      <c r="D51" s="1" t="s">
+      <c r="D51" t="s">
         <v>71</v>
       </c>
       <c r="E51">
@@ -1548,16 +1552,16 @@
       </c>
     </row>
     <row r="52" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="1" t="s">
+      <c r="A52" t="s">
         <v>60</v>
       </c>
-      <c r="B52" s="1" t="s">
+      <c r="B52" t="s">
         <v>75</v>
       </c>
-      <c r="C52" s="1" t="s">
+      <c r="C52" t="s">
         <v>60</v>
       </c>
-      <c r="D52" s="1" t="s">
+      <c r="D52" t="s">
         <v>75</v>
       </c>
       <c r="E52">
@@ -1565,16 +1569,16 @@
       </c>
     </row>
     <row r="53" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="1" t="s">
+      <c r="A53" t="s">
         <v>64</v>
       </c>
-      <c r="B53" s="1" t="s">
+      <c r="B53" t="s">
         <v>79</v>
       </c>
-      <c r="C53" s="1" t="s">
+      <c r="C53" t="s">
         <v>64</v>
       </c>
-      <c r="D53" s="1" t="s">
+      <c r="D53" t="s">
         <v>79</v>
       </c>
       <c r="E53">
@@ -1582,16 +1586,16 @@
       </c>
     </row>
     <row r="54" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="1" t="s">
+      <c r="A54" t="s">
         <v>68</v>
       </c>
-      <c r="B54" s="1" t="s">
+      <c r="B54" t="s">
         <v>83</v>
       </c>
-      <c r="C54" s="1" t="s">
+      <c r="C54" t="s">
         <v>68</v>
       </c>
-      <c r="D54" s="1" t="s">
+      <c r="D54" t="s">
         <v>83</v>
       </c>
       <c r="E54">
@@ -1599,16 +1603,16 @@
       </c>
     </row>
     <row r="55" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="1" t="s">
+      <c r="A55" t="s">
         <v>72</v>
       </c>
-      <c r="B55" s="1" t="s">
+      <c r="B55" t="s">
         <v>87</v>
       </c>
-      <c r="C55" s="1" t="s">
+      <c r="C55" t="s">
         <v>72</v>
       </c>
-      <c r="D55" s="1" t="s">
+      <c r="D55" t="s">
         <v>87</v>
       </c>
       <c r="E55">
@@ -1616,16 +1620,16 @@
       </c>
     </row>
     <row r="56" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="1" t="s">
+      <c r="A56" t="s">
         <v>76</v>
       </c>
-      <c r="B56" s="1" t="s">
+      <c r="B56" t="s">
         <v>91</v>
       </c>
-      <c r="C56" s="1" t="s">
+      <c r="C56" t="s">
         <v>76</v>
       </c>
-      <c r="D56" s="1" t="s">
+      <c r="D56" t="s">
         <v>91</v>
       </c>
       <c r="E56">
@@ -1633,16 +1637,16 @@
       </c>
     </row>
     <row r="57" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="1" t="s">
+      <c r="A57" t="s">
         <v>80</v>
       </c>
-      <c r="B57" s="1" t="s">
+      <c r="B57" t="s">
         <v>95</v>
       </c>
-      <c r="C57" s="1" t="s">
+      <c r="C57" t="s">
         <v>80</v>
       </c>
-      <c r="D57" s="1" t="s">
+      <c r="D57" t="s">
         <v>95</v>
       </c>
       <c r="E57">
@@ -1650,16 +1654,16 @@
       </c>
     </row>
     <row r="58" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="1" t="s">
+      <c r="A58" t="s">
         <v>84</v>
       </c>
-      <c r="B58" s="1" t="s">
+      <c r="B58" t="s">
         <v>97</v>
       </c>
-      <c r="C58" s="1" t="s">
+      <c r="C58" t="s">
         <v>84</v>
       </c>
-      <c r="D58" s="1" t="s">
+      <c r="D58" t="s">
         <v>97</v>
       </c>
       <c r="E58">
@@ -1667,16 +1671,16 @@
       </c>
     </row>
     <row r="59" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="1" t="s">
+      <c r="A59" t="s">
         <v>88</v>
       </c>
-      <c r="B59" s="1" t="s">
+      <c r="B59" t="s">
         <v>98</v>
       </c>
-      <c r="C59" s="1" t="s">
+      <c r="C59" t="s">
         <v>88</v>
       </c>
-      <c r="D59" s="1" t="s">
+      <c r="D59" t="s">
         <v>98</v>
       </c>
       <c r="E59">
@@ -1684,16 +1688,16 @@
       </c>
     </row>
     <row r="60" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="1" t="s">
+      <c r="A60" t="s">
         <v>92</v>
       </c>
-      <c r="B60" s="1" t="s">
+      <c r="B60" t="s">
         <v>96</v>
       </c>
-      <c r="C60" s="1" t="s">
+      <c r="C60" t="s">
         <v>92</v>
       </c>
-      <c r="D60" s="1" t="s">
+      <c r="D60" t="s">
         <v>96</v>
       </c>
       <c r="E60">
@@ -1701,16 +1705,16 @@
       </c>
     </row>
     <row r="61" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="1" t="s">
+      <c r="A61" t="s">
         <v>94</v>
       </c>
-      <c r="B61" s="1" t="s">
+      <c r="B61" t="s">
         <v>93</v>
       </c>
-      <c r="C61" s="1" t="s">
+      <c r="C61" t="s">
         <v>94</v>
       </c>
-      <c r="D61" s="1" t="s">
+      <c r="D61" t="s">
         <v>93</v>
       </c>
       <c r="E61">
@@ -1718,16 +1722,16 @@
       </c>
     </row>
     <row r="62" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="1" t="s">
+      <c r="A62" t="s">
         <v>90</v>
       </c>
-      <c r="B62" s="1" t="s">
+      <c r="B62" t="s">
         <v>89</v>
       </c>
-      <c r="C62" s="1" t="s">
+      <c r="C62" t="s">
         <v>90</v>
       </c>
-      <c r="D62" s="1" t="s">
+      <c r="D62" t="s">
         <v>89</v>
       </c>
       <c r="E62">
@@ -1735,16 +1739,16 @@
       </c>
     </row>
     <row r="63" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="1" t="s">
+      <c r="A63" t="s">
         <v>86</v>
       </c>
-      <c r="B63" s="1" t="s">
+      <c r="B63" t="s">
         <v>85</v>
       </c>
-      <c r="C63" s="1" t="s">
+      <c r="C63" t="s">
         <v>86</v>
       </c>
-      <c r="D63" s="1" t="s">
+      <c r="D63" t="s">
         <v>85</v>
       </c>
       <c r="E63">
@@ -1752,16 +1756,16 @@
       </c>
     </row>
     <row r="64" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="1" t="s">
+      <c r="A64" t="s">
         <v>82</v>
       </c>
-      <c r="B64" s="1" t="s">
+      <c r="B64" t="s">
         <v>81</v>
       </c>
-      <c r="C64" s="1" t="s">
+      <c r="C64" t="s">
         <v>82</v>
       </c>
-      <c r="D64" s="1" t="s">
+      <c r="D64" t="s">
         <v>81</v>
       </c>
       <c r="E64">
@@ -1769,16 +1773,16 @@
       </c>
     </row>
     <row r="65" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="1" t="s">
+      <c r="A65" t="s">
         <v>78</v>
       </c>
-      <c r="B65" s="1" t="s">
+      <c r="B65" t="s">
         <v>77</v>
       </c>
-      <c r="C65" s="1" t="s">
+      <c r="C65" t="s">
         <v>78</v>
       </c>
-      <c r="D65" s="1" t="s">
+      <c r="D65" t="s">
         <v>77</v>
       </c>
       <c r="E65">
@@ -1786,16 +1790,16 @@
       </c>
     </row>
     <row r="66" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="1" t="s">
+      <c r="A66" t="s">
         <v>74</v>
       </c>
-      <c r="B66" s="1" t="s">
+      <c r="B66" t="s">
         <v>73</v>
       </c>
-      <c r="C66" s="1" t="s">
+      <c r="C66" t="s">
         <v>74</v>
       </c>
-      <c r="D66" s="1" t="s">
+      <c r="D66" t="s">
         <v>73</v>
       </c>
       <c r="E66">
@@ -1803,16 +1807,16 @@
       </c>
     </row>
     <row r="67" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="1" t="s">
+      <c r="A67" t="s">
         <v>70</v>
       </c>
-      <c r="B67" s="1" t="s">
+      <c r="B67" t="s">
         <v>69</v>
       </c>
-      <c r="C67" s="1" t="s">
+      <c r="C67" t="s">
         <v>70</v>
       </c>
-      <c r="D67" s="1" t="s">
+      <c r="D67" t="s">
         <v>69</v>
       </c>
       <c r="E67">
@@ -1820,16 +1824,16 @@
       </c>
     </row>
     <row r="68" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="1" t="s">
+      <c r="A68" t="s">
         <v>66</v>
       </c>
-      <c r="B68" s="1" t="s">
+      <c r="B68" t="s">
         <v>65</v>
       </c>
-      <c r="C68" s="1" t="s">
+      <c r="C68" t="s">
         <v>66</v>
       </c>
-      <c r="D68" s="1" t="s">
+      <c r="D68" t="s">
         <v>65</v>
       </c>
       <c r="E68">
@@ -1837,16 +1841,16 @@
       </c>
     </row>
     <row r="69" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="1" t="s">
+      <c r="A69" t="s">
         <v>62</v>
       </c>
-      <c r="B69" s="1" t="s">
+      <c r="B69" t="s">
         <v>61</v>
       </c>
-      <c r="C69" s="1" t="s">
+      <c r="C69" t="s">
         <v>62</v>
       </c>
-      <c r="D69" s="1" t="s">
+      <c r="D69" t="s">
         <v>61</v>
       </c>
       <c r="E69">
@@ -1854,16 +1858,16 @@
       </c>
     </row>
     <row r="70" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="1" t="s">
+      <c r="A70" t="s">
         <v>58</v>
       </c>
-      <c r="B70" s="1" t="s">
+      <c r="B70" t="s">
         <v>57</v>
       </c>
-      <c r="C70" s="1" t="s">
+      <c r="C70" t="s">
         <v>58</v>
       </c>
-      <c r="D70" s="1" t="s">
+      <c r="D70" t="s">
         <v>57</v>
       </c>
       <c r="E70">
@@ -1871,16 +1875,16 @@
       </c>
     </row>
     <row r="71" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="1" t="s">
+      <c r="A71" t="s">
         <v>55</v>
       </c>
-      <c r="B71" s="1" t="s">
+      <c r="B71" t="s">
         <v>54</v>
       </c>
-      <c r="C71" s="1" t="s">
+      <c r="C71" t="s">
         <v>55</v>
       </c>
-      <c r="D71" s="1" t="s">
+      <c r="D71" t="s">
         <v>54</v>
       </c>
       <c r="E71">
@@ -1888,16 +1892,16 @@
       </c>
     </row>
     <row r="72" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="1" t="s">
+      <c r="A72" t="s">
         <v>53</v>
       </c>
-      <c r="B72" s="1" t="s">
+      <c r="B72" t="s">
         <v>52</v>
       </c>
-      <c r="C72" s="1" t="s">
+      <c r="C72" t="s">
         <v>53</v>
       </c>
-      <c r="D72" s="1" t="s">
+      <c r="D72" t="s">
         <v>52</v>
       </c>
       <c r="E72">
@@ -1905,16 +1909,16 @@
       </c>
     </row>
     <row r="73" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="1" t="s">
+      <c r="A73" t="s">
         <v>51</v>
       </c>
-      <c r="B73" s="1" t="s">
+      <c r="B73" t="s">
         <v>50</v>
       </c>
-      <c r="C73" s="1" t="s">
+      <c r="C73" t="s">
         <v>51</v>
       </c>
-      <c r="D73" s="1" t="s">
+      <c r="D73" t="s">
         <v>50</v>
       </c>
       <c r="E73">
@@ -1922,16 +1926,16 @@
       </c>
     </row>
     <row r="74" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="1" t="s">
+      <c r="A74" t="s">
         <v>49</v>
       </c>
-      <c r="B74" s="1" t="s">
+      <c r="B74" t="s">
         <v>48</v>
       </c>
-      <c r="C74" s="1" t="s">
+      <c r="C74" t="s">
         <v>99</v>
       </c>
-      <c r="D74" s="1" t="s">
+      <c r="D74" t="s">
         <v>48</v>
       </c>
       <c r="E74">
@@ -1939,16 +1943,16 @@
       </c>
     </row>
     <row r="75" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="1" t="s">
+      <c r="A75" t="s">
         <v>47</v>
       </c>
-      <c r="B75" s="1" t="s">
+      <c r="B75" t="s">
         <v>46</v>
       </c>
-      <c r="C75" s="1" t="s">
+      <c r="C75" t="s">
         <v>5</v>
       </c>
-      <c r="D75" s="1" t="s">
+      <c r="D75" t="s">
         <v>46</v>
       </c>
       <c r="E75">
@@ -1956,16 +1960,16 @@
       </c>
     </row>
     <row r="76" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="1" t="s">
+      <c r="A76" t="s">
         <v>45</v>
       </c>
-      <c r="B76" s="1" t="s">
+      <c r="B76" t="s">
         <v>44</v>
       </c>
-      <c r="C76" s="1" t="s">
+      <c r="C76" t="s">
         <v>7</v>
       </c>
-      <c r="D76" s="1" t="s">
+      <c r="D76" t="s">
         <v>44</v>
       </c>
       <c r="E76">
@@ -1973,16 +1977,16 @@
       </c>
     </row>
     <row r="77" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="1" t="s">
+      <c r="A77" t="s">
         <v>43</v>
       </c>
-      <c r="B77" s="1" t="s">
+      <c r="B77" t="s">
         <v>42</v>
       </c>
-      <c r="C77" s="1" t="s">
+      <c r="C77" t="s">
         <v>9</v>
       </c>
-      <c r="D77" s="1" t="s">
+      <c r="D77" t="s">
         <v>42</v>
       </c>
       <c r="E77">
@@ -1990,16 +1994,16 @@
       </c>
     </row>
     <row r="78" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="1" t="s">
+      <c r="A78" t="s">
         <v>41</v>
       </c>
-      <c r="B78" s="1" t="s">
+      <c r="B78" t="s">
         <v>40</v>
       </c>
-      <c r="C78" s="1" t="s">
+      <c r="C78" t="s">
         <v>11</v>
       </c>
-      <c r="D78" s="1" t="s">
+      <c r="D78" t="s">
         <v>40</v>
       </c>
       <c r="E78">
@@ -2007,16 +2011,16 @@
       </c>
     </row>
     <row r="79" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="1" t="s">
+      <c r="A79" t="s">
         <v>39</v>
       </c>
-      <c r="B79" s="1" t="s">
+      <c r="B79" t="s">
         <v>38</v>
       </c>
-      <c r="C79" s="1" t="s">
+      <c r="C79" t="s">
         <v>13</v>
       </c>
-      <c r="D79" s="1" t="s">
+      <c r="D79" t="s">
         <v>38</v>
       </c>
       <c r="E79">
@@ -2024,16 +2028,16 @@
       </c>
     </row>
     <row r="80" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="1" t="s">
+      <c r="A80" t="s">
         <v>37</v>
       </c>
-      <c r="B80" s="1" t="s">
+      <c r="B80" t="s">
         <v>36</v>
       </c>
-      <c r="C80" s="1" t="s">
+      <c r="C80" t="s">
         <v>15</v>
       </c>
-      <c r="D80" s="1" t="s">
+      <c r="D80" t="s">
         <v>36</v>
       </c>
       <c r="E80">
@@ -2041,16 +2045,16 @@
       </c>
     </row>
     <row r="81" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A81" s="1" t="s">
+      <c r="A81" t="s">
         <v>35</v>
       </c>
-      <c r="B81" s="1" t="s">
+      <c r="B81" t="s">
         <v>34</v>
       </c>
-      <c r="C81" s="1" t="s">
+      <c r="C81" t="s">
         <v>17</v>
       </c>
-      <c r="D81" s="1" t="s">
+      <c r="D81" t="s">
         <v>34</v>
       </c>
       <c r="E81">
@@ -2058,16 +2062,16 @@
       </c>
     </row>
     <row r="82" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A82" s="1" t="s">
+      <c r="A82" t="s">
         <v>33</v>
       </c>
-      <c r="B82" s="1" t="s">
+      <c r="B82" t="s">
         <v>32</v>
       </c>
-      <c r="C82" s="1" t="s">
+      <c r="C82" t="s">
         <v>19</v>
       </c>
-      <c r="D82" s="1" t="s">
+      <c r="D82" t="s">
         <v>32</v>
       </c>
       <c r="E82">
@@ -2075,16 +2079,16 @@
       </c>
     </row>
     <row r="83" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A83" s="1" t="s">
+      <c r="A83" t="s">
         <v>31</v>
       </c>
-      <c r="B83" s="1" t="s">
+      <c r="B83" t="s">
         <v>30</v>
       </c>
-      <c r="C83" s="1" t="s">
+      <c r="C83" t="s">
         <v>21</v>
       </c>
-      <c r="D83" s="1" t="s">
+      <c r="D83" t="s">
         <v>30</v>
       </c>
       <c r="E83">
@@ -2092,16 +2096,16 @@
       </c>
     </row>
     <row r="84" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A84" s="1" t="s">
+      <c r="A84" t="s">
         <v>29</v>
       </c>
-      <c r="B84" s="1" t="s">
+      <c r="B84" t="s">
         <v>28</v>
       </c>
-      <c r="C84" s="1" t="s">
+      <c r="C84" t="s">
         <v>23</v>
       </c>
-      <c r="D84" s="1" t="s">
+      <c r="D84" t="s">
         <v>28</v>
       </c>
       <c r="E84">
@@ -2109,16 +2113,16 @@
       </c>
     </row>
     <row r="85" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A85" s="1" t="s">
+      <c r="A85" t="s">
         <v>27</v>
       </c>
-      <c r="B85" s="1" t="s">
+      <c r="B85" t="s">
         <v>26</v>
       </c>
-      <c r="C85" s="1" t="s">
+      <c r="C85" t="s">
         <v>25</v>
       </c>
-      <c r="D85" s="1" t="s">
+      <c r="D85" t="s">
         <v>26</v>
       </c>
       <c r="E85">
@@ -2126,16 +2130,16 @@
       </c>
     </row>
     <row r="86" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A86" s="1" t="s">
+      <c r="A86" t="s">
         <v>25</v>
       </c>
-      <c r="B86" s="1" t="s">
+      <c r="B86" t="s">
         <v>24</v>
       </c>
-      <c r="C86" s="1" t="s">
+      <c r="C86" t="s">
         <v>27</v>
       </c>
-      <c r="D86" s="1" t="s">
+      <c r="D86" t="s">
         <v>24</v>
       </c>
       <c r="E86">
@@ -2143,16 +2147,16 @@
       </c>
     </row>
     <row r="87" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A87" s="1" t="s">
+      <c r="A87" t="s">
         <v>23</v>
       </c>
-      <c r="B87" s="1" t="s">
+      <c r="B87" t="s">
         <v>22</v>
       </c>
-      <c r="C87" s="1" t="s">
+      <c r="C87" t="s">
         <v>29</v>
       </c>
-      <c r="D87" s="1" t="s">
+      <c r="D87" t="s">
         <v>22</v>
       </c>
       <c r="E87">
@@ -2160,16 +2164,16 @@
       </c>
     </row>
     <row r="88" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A88" s="1" t="s">
+      <c r="A88" t="s">
         <v>21</v>
       </c>
-      <c r="B88" s="1" t="s">
+      <c r="B88" t="s">
         <v>20</v>
       </c>
-      <c r="C88" s="1" t="s">
+      <c r="C88" t="s">
         <v>31</v>
       </c>
-      <c r="D88" s="1" t="s">
+      <c r="D88" t="s">
         <v>20</v>
       </c>
       <c r="E88">
@@ -2177,16 +2181,16 @@
       </c>
     </row>
     <row r="89" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A89" s="1" t="s">
+      <c r="A89" t="s">
         <v>19</v>
       </c>
-      <c r="B89" s="1" t="s">
+      <c r="B89" t="s">
         <v>18</v>
       </c>
-      <c r="C89" s="1" t="s">
+      <c r="C89" t="s">
         <v>33</v>
       </c>
-      <c r="D89" s="1" t="s">
+      <c r="D89" t="s">
         <v>18</v>
       </c>
       <c r="E89">
@@ -2194,16 +2198,16 @@
       </c>
     </row>
     <row r="90" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A90" s="1" t="s">
+      <c r="A90" t="s">
         <v>17</v>
       </c>
-      <c r="B90" s="1" t="s">
+      <c r="B90" t="s">
         <v>16</v>
       </c>
-      <c r="C90" s="1" t="s">
+      <c r="C90" t="s">
         <v>35</v>
       </c>
-      <c r="D90" s="1" t="s">
+      <c r="D90" t="s">
         <v>16</v>
       </c>
       <c r="E90">
@@ -2211,16 +2215,16 @@
       </c>
     </row>
     <row r="91" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A91" s="1" t="s">
+      <c r="A91" t="s">
         <v>15</v>
       </c>
-      <c r="B91" s="1" t="s">
+      <c r="B91" t="s">
         <v>14</v>
       </c>
-      <c r="C91" s="1" t="s">
+      <c r="C91" t="s">
         <v>37</v>
       </c>
-      <c r="D91" s="1" t="s">
+      <c r="D91" t="s">
         <v>14</v>
       </c>
       <c r="E91">
@@ -2228,16 +2232,16 @@
       </c>
     </row>
     <row r="92" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A92" s="1" t="s">
+      <c r="A92" t="s">
         <v>13</v>
       </c>
-      <c r="B92" s="1" t="s">
+      <c r="B92" t="s">
         <v>12</v>
       </c>
-      <c r="C92" s="1" t="s">
+      <c r="C92" t="s">
         <v>39</v>
       </c>
-      <c r="D92" s="1" t="s">
+      <c r="D92" t="s">
         <v>12</v>
       </c>
       <c r="E92">
@@ -2245,16 +2249,16 @@
       </c>
     </row>
     <row r="93" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A93" s="1" t="s">
+      <c r="A93" t="s">
         <v>11</v>
       </c>
-      <c r="B93" s="1" t="s">
+      <c r="B93" t="s">
         <v>10</v>
       </c>
-      <c r="C93" s="1" t="s">
+      <c r="C93" t="s">
         <v>41</v>
       </c>
-      <c r="D93" s="1" t="s">
+      <c r="D93" t="s">
         <v>10</v>
       </c>
       <c r="E93">
@@ -2262,16 +2266,16 @@
       </c>
     </row>
     <row r="94" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A94" s="1" t="s">
+      <c r="A94" t="s">
         <v>9</v>
       </c>
-      <c r="B94" s="1" t="s">
+      <c r="B94" t="s">
         <v>8</v>
       </c>
-      <c r="C94" s="1" t="s">
+      <c r="C94" t="s">
         <v>43</v>
       </c>
-      <c r="D94" s="1" t="s">
+      <c r="D94" t="s">
         <v>8</v>
       </c>
       <c r="E94">
@@ -2279,16 +2283,16 @@
       </c>
     </row>
     <row r="95" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A95" s="1" t="s">
+      <c r="A95" t="s">
         <v>7</v>
       </c>
-      <c r="B95" s="1" t="s">
+      <c r="B95" t="s">
         <v>6</v>
       </c>
-      <c r="C95" s="1" t="s">
+      <c r="C95" t="s">
         <v>45</v>
       </c>
-      <c r="D95" s="1" t="s">
+      <c r="D95" t="s">
         <v>6</v>
       </c>
       <c r="E95">
@@ -2296,16 +2300,16 @@
       </c>
     </row>
     <row r="96" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A96" s="1" t="s">
+      <c r="A96" t="s">
         <v>5</v>
       </c>
-      <c r="B96" s="1" t="s">
+      <c r="B96" t="s">
         <v>4</v>
       </c>
-      <c r="C96" s="1" t="s">
+      <c r="C96" t="s">
         <v>47</v>
       </c>
-      <c r="D96" s="1" t="s">
+      <c r="D96" t="s">
         <v>4</v>
       </c>
       <c r="E96">

</xml_diff>